<commit_message>
Agrego ruta POST /api/estadisticas para cargar estadísticas
</commit_message>
<xml_diff>
--- a/uploads/eventos/base_eventos.xlsx
+++ b/uploads/eventos/base_eventos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fab9de1464581e56/Documentos/Mapa_riesgos_Cauca/riesgo-despachos/backend/uploads/eventos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{804169EE-579C-4717-A7D0-741AC04D43E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5A61DA9-DA13-4900-88DF-0B0822724631}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{804169EE-579C-4717-A7D0-741AC04D43E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B941FEE-54D8-435D-BD46-0EF6EAE7CBD0}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -161,6 +161,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -458,7 +462,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="13.26953125" customWidth="1"/>
+    <col min="1" max="1" width="14.6328125" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" customWidth="1"/>
     <col min="4" max="4" width="12.7265625" customWidth="1"/>
     <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.90625" bestFit="1" customWidth="1"/>

</xml_diff>